<commit_message>
0.99 update tournament analysis tab
</commit_message>
<xml_diff>
--- a/GRONESTATS 1.0/Liga 1 Peru/2_Matches_Detailed.xlsx
+++ b/GRONESTATS 1.0/Liga 1 Peru/2_Matches_Detailed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStats\GRONESTATS 1.0\Liga 1 Peru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C85C1E3-C8A6-4B38-BB10-442C4A6FD59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5CE74A-BF57-48B3-A484-0B8CE575A211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -6322,7 +6322,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="346">
+  <dxfs count="174">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -7340,6 +7340,20 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <bgColor theme="6" tint="-0.249977111117893"/>
         </patternFill>
@@ -7354,8 +7368,22 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39997558519241921"/>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7363,13 +7391,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7390,28 +7411,21 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <bgColor theme="6" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5"/>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7452,27 +7466,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <bgColor theme="9" tint="0.39997558519241921"/>
         </patternFill>
@@ -7481,98 +7474,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.249977111117893"/>
+          <bgColor theme="5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7606,70 +7508,7 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <bgColor theme="6" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
@@ -7683,83 +7522,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39997558519241921"/>
         </patternFill>
@@ -7768,973 +7530,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="6" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
@@ -26706,7 +25502,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BB1D9A8-5F5F-43AC-9B4B-13392B01CB03}" name="TablaDinámica1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Dificultad total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BB1D9A8-5F5F-43AC-9B4B-13392B01CB03}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Dificultad total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:N104" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -27149,7 +25945,7 @@
     <dataField name="Suma de pain_points" fld="13" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="29">
-    <format dxfId="0">
+    <format dxfId="173">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27158,7 +25954,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="172">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27167,7 +25963,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="171">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27176,7 +25972,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="170">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27185,7 +25981,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="169">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27194,7 +25990,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="168">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27203,7 +25999,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="167">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27212,7 +26008,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="166">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27221,7 +26017,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="165">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27230,7 +26026,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="164">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27239,7 +26035,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="163">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27248,7 +26044,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="162">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27257,7 +26053,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="161">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27266,7 +26062,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="160">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27275,7 +26071,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="159">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27284,7 +26080,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="158">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27293,7 +26089,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="157">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27302,7 +26098,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="156">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27311,7 +26107,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="155">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27320,7 +26116,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="154">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27329,7 +26125,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="153">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27338,7 +26134,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="152">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27347,7 +26143,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="151">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27356,7 +26152,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="150">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27365,7 +26161,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="149">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27374,7 +26170,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="148">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27383,7 +26179,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="147">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27392,7 +26188,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="146">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -27401,7 +26197,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="145">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -78456,8 +77252,8 @@
   <dimension ref="A1:O104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O96" sqref="O96"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -78475,7 +77271,7 @@
     <col min="11" max="11" width="28.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="33.21875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23" bestFit="1" customWidth="1"/>
@@ -81892,7 +80688,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting pivot="1" sqref="N12 N8 N16 N20 N24 N28 N32 N36 N40 N44 N48 N52 N56 N60 N64 N68 N72 N76 N80 N84 N88 N92 N96 N100 M12 M8 M16 M20 M24 M28 M32 M36 M40 M44 M48 M52 M56 M60 M64 M68 M72 M76 M80 M84 M88 M92 M96 M100 F12 F8 F16 F20 F24 F28 F32 F36 F40 F44 F48 F52 F56 F60 F64 F68 F72 F76 F80 F84 F88 F92 F96 F100 J12 J8 J16 J20 J24 J28 J32 J36 J40 J44 J48 J52 J56 J60 J64 J68 J72 J76 J80 J84 J88 J92 J96 J100">
+  <conditionalFormatting pivot="1" sqref="N8 N12 N16 N20 N24 N28 N32 N36 N40 N44 N48 N52 N56 N60 N64 N68 N72 N76 N80 N84 N88 N92 N96 N100 M12 M8 M16 M20 M24 M28 M32 M36 M40 M44 M48 M52 M56 M60 M64 M68 M72 M76 M80 M84 M88 M92 M96 M100 F12 F8 F16 F20 F24 F28 F32 F36 F40 F44 F48 F52 F56 F60 F64 F68 F72 F76 F80 F84 F88 F92 F96 F100 J12 J8 J16 J20 J24 J28 J32 J36 J40 J44 J48 J52 J56 J60 J64 J68 J72 J76 J80 J84 J88 J92 J96 J100">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>